<commit_message>
with working test on off seperate code
</commit_message>
<xml_diff>
--- a/Philips Sensor Connections.xlsx
+++ b/Philips Sensor Connections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anish\OneDrive\Desktop\Philips Demo 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/87673216a5f8eb71/Desktop/dev/Philips-Esp32-Development/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE6AAE2-2CD9-4E4E-AFE3-7ECE8DC474AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{86D9ADE2-1F4C-442A-AD66-F3B5E0C4FE99}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{86D9ADE2-1F4C-442A-AD66-F3B5E0C4FE99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,7 +414,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:I18"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,20 +792,36 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="E31:I31"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="E3:I3"/>
@@ -822,39 +838,23 @@
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="E8:I8"/>
     <mergeCell ref="E9:I9"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E30:I30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>